<commit_message>
Updated for total population
</commit_message>
<xml_diff>
--- a/answer.xlsx
+++ b/answer.xlsx
@@ -15,15 +15,15 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="results" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>Year</t>
   </si>
@@ -31,10 +31,34 @@
     <t>Group</t>
   </si>
   <si>
-    <t>other occupation</t>
+    <t>Engineering</t>
   </si>
   <si>
-    <t>Science</t>
+    <t>Math and Computational Science</t>
+  </si>
+  <si>
+    <t>Natural Science</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Post-Secondary Teachers</t>
+  </si>
+  <si>
+    <t>Blue Collar</t>
+  </si>
+  <si>
+    <t>Other Occupation</t>
+  </si>
+  <si>
+    <t>Hispanic Descendant</t>
+  </si>
+  <si>
+    <t>Direct Hispanic Immigrant</t>
+  </si>
+  <si>
+    <t>Chinese Descendant</t>
   </si>
   <si>
     <t>Direct Chinese Immigrant</t>
@@ -43,13 +67,7 @@
     <t>Vanilla</t>
   </si>
   <si>
-    <t>Chinese Descendant</t>
-  </si>
-  <si>
-    <t>Hispanic Descendant</t>
-  </si>
-  <si>
-    <t>Direct Hispanic Immigrant</t>
+    <t>Total</t>
   </si>
   <si>
     <t>Row Labels</t>
@@ -58,10 +76,10 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Sum of Science</t>
+    <t>Column Labels</t>
   </si>
   <si>
-    <t>Column Labels</t>
+    <t>Sum of Engineering</t>
   </si>
 </sst>
 </file>
@@ -501,8 +519,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -545,57 +564,60 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,6 +683,21 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
           <a:solidFill>
@@ -678,6 +715,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -705,6 +745,155 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -730,11 +919,14 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="6"/>
+        <c:idx val="11"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -745,11 +937,11 @@
           <c:size val="5"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln w="9525">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -757,11 +949,13 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="7"/>
+        <c:idx val="12"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -772,11 +966,11 @@
           <c:size val="5"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln w="9525">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -784,11 +978,11 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="8"/>
+        <c:idx val="13"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -799,11 +993,206 @@
           <c:size val="5"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln w="9525">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -821,7 +1210,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$B$4</c:f>
+              <c:f>Sheet1!$B$4:$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -833,7 +1222,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -844,11 +1235,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -856,7 +1251,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>Sheet1!$A$6:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -876,7 +1271,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$9</c:f>
+              <c:f>Sheet1!$B$6:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -884,13 +1279,13 @@
                   <c:v>5.2631578947368397E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22267871815940801</c:v>
+                  <c:v>4.1906327033689302E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22991689750692501</c:v>
+                  <c:v>5.8171745152354501E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.256354916067146</c:v>
+                  <c:v>2.90167865707434E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -902,7 +1297,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$3:$C$4</c:f>
+              <c:f>Sheet1!$C$4:$C$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -937,7 +1332,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>Sheet1!$A$6:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -957,21 +1352,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$9</c:f>
+              <c:f>Sheet1!$C$6:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.215053763440859</c:v>
+                  <c:v>5.3763440860214902E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10913500404203701</c:v>
+                  <c:v>5.86095392077607E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25889594152721601</c:v>
+                  <c:v>6.4243123677630201E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25489675516224197</c:v>
+                  <c:v>5.0412979351032401E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -983,7 +1378,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$3:$D$4</c:f>
+              <c:f>Sheet1!$D$4:$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -995,7 +1390,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1006,11 +1404,17 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1018,7 +1422,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>Sheet1!$A$6:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1038,21 +1442,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$9</c:f>
+              <c:f>Sheet1!$D$6:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.20481927710844E-2</c:v>
+                  <c:v>2.4096385542168798E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2454245765601797E-2</c:v>
+                  <c:v>4.8880300102307501E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5519152072795599E-2</c:v>
+                  <c:v>2.5671656965660901E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2189234324657199E-2</c:v>
+                  <c:v>2.0512474485923E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1064,7 +1468,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$3:$E$4</c:f>
+              <c:f>Sheet1!$E$4:$E$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1076,7 +1480,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1087,11 +1493,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1099,7 +1509,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>Sheet1!$A$6:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1119,21 +1529,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$9</c:f>
+              <c:f>Sheet1!$E$6:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.90102389078498E-2</c:v>
+                  <c:v>8.5324232081911405E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2292162749767E-2</c:v>
+                  <c:v>9.2142043689822893E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8128342245989199E-2</c:v>
+                  <c:v>5.4140233168366103E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9482872314580102E-2</c:v>
+                  <c:v>7.4272029986464398E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1145,7 +1555,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$3:$F$4</c:f>
+              <c:f>Sheet1!$F$4:$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1157,7 +1567,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1168,11 +1578,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent5"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1180,7 +1590,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>Sheet1!$A$6:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1200,21 +1610,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$F$9</c:f>
+              <c:f>Sheet1!$F$6:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.9629248197713702E-2</c:v>
+                  <c:v>1.59629248197674E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.1468297581152695E-2</c:v>
+                  <c:v>1.5999741847800501E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.5853952535626402E-2</c:v>
+                  <c:v>1.51227615776199E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.13973065688815E-2</c:v>
+                  <c:v>1.1792474943997201E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1231,11 +1641,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="555196528"/>
-        <c:axId val="555195440"/>
+        <c:axId val="1047385152"/>
+        <c:axId val="1047379712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="555196528"/>
+        <c:axId val="1047385152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1688,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="555195440"/>
+        <c:crossAx val="1047379712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1286,7 +1696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="555195440"/>
+        <c:axId val="1047379712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1747,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="555196528"/>
+        <c:crossAx val="1047385152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1976,16 +2386,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2008,33 +2418,92 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Aryan" refreshedDate="41759.659441898148" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="20">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Aryan" refreshedDate="41759.775790624997" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="20">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:D21" sheet="results"/>
+    <worksheetSource ref="A1:J21" sheet="results"/>
   </cacheSource>
-  <cacheFields count="4">
+  <cacheFields count="10">
     <cacheField name="Year" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1980" maxValue="2010" count="4">
         <n v="2000"/>
         <n v="2010"/>
+        <n v="1990"/>
         <n v="1980"/>
-        <n v="1990"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Group" numFmtId="0">
       <sharedItems count="5">
+        <s v="Hispanic Descendant"/>
+        <s v="Direct Hispanic Immigrant"/>
+        <s v="Chinese Descendant"/>
         <s v="Direct Chinese Immigrant"/>
         <s v="Vanilla"/>
-        <s v="Chinese Descendant"/>
-        <s v="Hispanic Descendant"/>
-        <s v="Direct Hispanic Immigrant"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="other occupation" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.74110405847278304" maxValue="0.98795180722891496"/>
+    <cacheField name="Engineering" numFmtId="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.0512474485923E-3" maxValue="6.4243123677630201E-2" count="20">
+        <n v="5.4140233168366103E-3"/>
+        <n v="2.5671656965660901E-3"/>
+        <n v="5.8171745152354501E-2"/>
+        <n v="6.4243123677630201E-2"/>
+        <n v="1.51227615776199E-2"/>
+        <n v="7.4272029986464398E-3"/>
+        <n v="2.0512474485923E-3"/>
+        <n v="5.0412979351032401E-2"/>
+        <n v="2.90167865707434E-2"/>
+        <n v="1.1792474943997201E-2"/>
+        <n v="9.2142043689822893E-3"/>
+        <n v="4.8880300102307501E-3"/>
+        <n v="4.1906327033689302E-2"/>
+        <n v="5.86095392077607E-2"/>
+        <n v="1.5999741847800501E-2"/>
+        <n v="8.5324232081911405E-3"/>
+        <n v="2.4096385542168798E-3"/>
+        <n v="5.3763440860214902E-2"/>
+        <n v="5.2631578947368397E-2"/>
+        <n v="1.59629248197674E-2"/>
+      </sharedItems>
     </cacheField>
-    <cacheField name="Science" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.20481927710844E-2" maxValue="0.25889594152721601"/>
+    <cacheField name="Math and Computational Science" numFmtId="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="7.9136690647481994E-2" count="19">
+        <n v="9.6655262895672008E-3"/>
+        <n v="3.50761253590219E-3"/>
+        <n v="5.5401662049861501E-2"/>
+        <n v="5.94345066358914E-2"/>
+        <n v="1.69499283819281E-2"/>
+        <n v="1.41646131954326E-2"/>
+        <n v="3.0802449351394201E-3"/>
+        <n v="2.68141592920354E-2"/>
+        <n v="7.9136690647481994E-2"/>
+        <n v="1.8125931255745398E-2"/>
+        <n v="3.0541463919660401E-3"/>
+        <n v="1.9324769807889E-3"/>
+        <n v="3.04026294165981E-2"/>
+        <n v="2.5869037995149499E-2"/>
+        <n v="8.5304116578497503E-3"/>
+        <n v="1.7064846416382201E-3"/>
+        <n v="0"/>
+        <n v="2.1505376344085898E-2"/>
+        <n v="4.3769309989685297E-3"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Natural Science" numFmtId="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="6.5204847085977999E-2"/>
+    </cacheField>
+    <cacheField name="Health" numFmtId="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="9.2851273623664701E-2"/>
+    </cacheField>
+    <cacheField name="Post-Secondary Teachers" numFmtId="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="4.0407673860911202E-2"/>
+    </cacheField>
+    <cacheField name="Blue Collar" numFmtId="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.1942446043165399E-2" maxValue="0.56144578313253102"/>
+    </cacheField>
+    <cacheField name="Other Occupation" numFmtId="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.42063391200467698" maxValue="0.89473684210526305"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="10">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.99999999999969069" maxValue="1.000000000000052"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -2050,134 +2519,254 @@
   <r>
     <x v="0"/>
     <x v="0"/>
-    <n v="0.74110405847278304"/>
-    <n v="0.25889594152721601"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2.12575148636529E-3"/>
+    <n v="2.2552894675656798E-2"/>
+    <n v="6.8422625967382899E-3"/>
+    <n v="0.27398943767230099"/>
+    <n v="0.67941010396253398"/>
+    <n v="0.99999999999999911"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
-    <n v="0.91414604746440398"/>
-    <n v="8.5853952535626402E-2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="9.4044683933609396E-4"/>
+    <n v="1.29629158935515E-2"/>
+    <n v="2.8213405180082798E-3"/>
+    <n v="0.556566606511958"/>
+    <n v="0.42063391200467698"/>
+    <n v="0.99999999999999911"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
-    <n v="0.77008310249307399"/>
-    <n v="0.22991689750692501"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3.7857802400738598E-2"/>
+    <n v="7.8485687903970397E-2"/>
+    <n v="0"/>
+    <n v="0.140350877192982"/>
+    <n v="0.62973222530009199"/>
+    <n v="0.999999999999999"/>
   </r>
   <r>
     <x v="0"/>
     <x v="3"/>
-    <n v="0.95187165775401095"/>
-    <n v="4.8128342245989199E-2"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="6.5204847085977999E-2"/>
+    <n v="3.1159838430467299E-2"/>
+    <n v="3.5391421427197499E-2"/>
+    <n v="0.129832660126947"/>
+    <n v="0.61473360261588705"/>
+    <n v="0.99999999999999845"/>
   </r>
   <r>
     <x v="0"/>
     <x v="4"/>
-    <n v="0.97448084792720402"/>
-    <n v="2.5519152072795599E-2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="4.8864314745695799E-3"/>
+    <n v="3.8641335548313699E-2"/>
+    <n v="7.4269180960085598E-3"/>
+    <n v="0.25538947452743299"/>
+    <n v="0.66158315039417903"/>
+    <n v="1.000000000000052"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="2.2255579078887902E-3"/>
+    <n v="1.8611390691701601E-2"/>
+    <n v="3.4576406483184598E-3"/>
+    <n v="0.24626904522264201"/>
+    <n v="0.70784454933537"/>
+    <n v="0.99999999999999989"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="2.1996929876351599E-3"/>
+    <n v="1.04350466422631E-2"/>
+    <n v="2.7226261365361601E-3"/>
+    <n v="0.48588249186080001"/>
+    <n v="0.49362864998903599"/>
+    <n v="1.0000000000000022"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="7"/>
+    <x v="7"/>
+    <n v="6.2743362831858399E-2"/>
+    <n v="7.2654867256637196E-2"/>
+    <n v="3.88200589970501E-2"/>
+    <n v="0.102300884955752"/>
+    <n v="0.64625368731563404"/>
+    <n v="0.99999999999999956"/>
   </r>
   <r>
     <x v="1"/>
     <x v="2"/>
-    <n v="0.743645083932853"/>
-    <n v="0.256354916067146"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="0.918602693431118"/>
-    <n v="8.13973065688815E-2"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0.74510324483775703"/>
-    <n v="0.25489675516224197"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="3"/>
-    <n v="0.95051712768541996"/>
-    <n v="4.9482872314580102E-2"/>
+    <x v="8"/>
+    <x v="8"/>
+    <n v="1.45083932853717E-2"/>
+    <n v="8.7170263788968805E-2"/>
+    <n v="4.0407673860911202E-2"/>
+    <n v="2.1942446043165399E-2"/>
+    <n v="0.72781774580335701"/>
+    <n v="0.99999999999999956"/>
   </r>
   <r>
     <x v="1"/>
     <x v="4"/>
-    <n v="0.97781076567534297"/>
-    <n v="2.2189234324657199E-2"/>
+    <x v="9"/>
+    <x v="9"/>
+    <n v="4.04157349862718E-3"/>
+    <n v="3.7328093501643698E-2"/>
+    <n v="7.5637840118548197E-3"/>
+    <n v="0.23254090391173199"/>
+    <n v="0.68860723887639297"/>
+    <n v="0.99999999999999323"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="10"/>
+    <n v="3.7270939020602502E-3"/>
+    <n v="1.6150740242261E-2"/>
+    <n v="6.9883010663629704E-3"/>
+    <n v="0.32767367222279697"/>
+    <n v="0.63319184180556898"/>
+    <n v="0.99999999999999845"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="11"/>
+    <n v="7.4457201318631197E-3"/>
+    <n v="1.4209389564624199E-2"/>
+    <n v="5.1153802432647396E-4"/>
+    <n v="0.52728202796407697"/>
+    <n v="0.44373081732408698"/>
+    <n v="0.99999999999999734"/>
   </r>
   <r>
     <x v="2"/>
     <x v="2"/>
-    <n v="0.94736842105263097"/>
-    <n v="5.2631578947368397E-2"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="0.94037075180224305"/>
-    <n v="5.9629248197713702E-2"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0.78494623655913898"/>
-    <n v="0.215053763440859"/>
+    <x v="12"/>
+    <x v="12"/>
+    <n v="2.3829087921117501E-2"/>
+    <n v="9.2851273623664701E-2"/>
+    <n v="3.3689400164338502E-2"/>
+    <n v="4.51930977814297E-2"/>
+    <n v="0.73212818405916102"/>
+    <n v="0.99999999999999889"/>
   </r>
   <r>
     <x v="2"/>
     <x v="3"/>
-    <n v="0.97098976109214796"/>
-    <n v="2.90102389078498E-2"/>
+    <x v="13"/>
+    <x v="13"/>
+    <n v="2.8294260307194798E-3"/>
+    <n v="1.4955537590945801E-2"/>
+    <n v="6.8714632174616003E-3"/>
+    <n v="0.22837510105092901"/>
+    <n v="0.66248989490703303"/>
+    <n v="0.99999999999999911"/>
   </r>
   <r>
     <x v="2"/>
     <x v="4"/>
-    <n v="0.98795180722891496"/>
-    <n v="1.20481927710844E-2"/>
+    <x v="14"/>
+    <x v="14"/>
+    <n v="3.84001397058968E-3"/>
+    <n v="3.2124763439574801E-2"/>
+    <n v="6.0836602944834102E-3"/>
+    <n v="0.27618678830190801"/>
+    <n v="0.65723462048779602"/>
+    <n v="1.0000000000000022"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
-    <n v="0.89086499595796298"/>
-    <n v="0.10913500404203701"/>
+    <x v="15"/>
+    <x v="15"/>
+    <n v="0"/>
+    <n v="1.0238907849829299E-2"/>
+    <n v="6.8259385665529098E-3"/>
+    <n v="0.42832764505119297"/>
+    <n v="0.54436860068259096"/>
+    <n v="0.99999999999999556"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
-    <n v="0.92853170241884198"/>
-    <n v="7.1468297581152695E-2"/>
+    <x v="16"/>
+    <x v="16"/>
+    <n v="0"/>
+    <n v="7.2289156626506503E-3"/>
+    <n v="0"/>
+    <n v="0.56144578313253102"/>
+    <n v="0.42891566265060399"/>
+    <n v="1.0000000000000027"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="17"/>
+    <n v="5.3763440860214902E-2"/>
+    <n v="4.3010752688171901E-2"/>
+    <n v="2.1505376344085898E-2"/>
+    <n v="0.18279569892472999"/>
+    <n v="0.62365591397849396"/>
+    <n v="0.99999999999999745"/>
   </r>
   <r>
     <x v="3"/>
     <x v="2"/>
-    <n v="0.77732128184059102"/>
-    <n v="0.22267871815940801"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <n v="0.95770783725023201"/>
-    <n v="4.2292162749767E-2"/>
+    <x v="18"/>
+    <x v="16"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5.2631578947368397E-2"/>
+    <n v="0.89473684210526305"/>
+    <n v="0.99999999999999989"/>
   </r>
   <r>
     <x v="3"/>
     <x v="4"/>
-    <n v="0.96754575423439804"/>
-    <n v="3.2454245765601797E-2"/>
+    <x v="19"/>
+    <x v="18"/>
+    <n v="3.2440782698237298E-3"/>
+    <n v="2.6210092687940698E-2"/>
+    <n v="8.1359423274944397E-3"/>
+    <n v="0.310092687950418"/>
+    <n v="0.63197734294527796"/>
+    <n v="0.99999999999969069"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
-  <location ref="A3:G9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="A4:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
+        <item x="3"/>
         <item x="2"/>
-        <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
@@ -2186,15 +2775,68 @@
     <pivotField axis="axisCol" showAll="0">
       <items count="6">
         <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
         <item x="0"/>
         <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="10" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="21">
+        <item x="6"/>
+        <item x="16"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="15"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="19"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="12"/>
+        <item x="7"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="10" showAll="0">
+      <items count="20">
+        <item x="16"/>
+        <item x="15"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="18"/>
+        <item x="14"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="9"/>
+        <item x="17"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="10" showAll="0"/>
+    <pivotField numFmtId="10" showAll="0"/>
+    <pivotField numFmtId="10" showAll="0"/>
+    <pivotField numFmtId="10" showAll="0"/>
+    <pivotField numFmtId="10" showAll="0"/>
+    <pivotField numFmtId="10" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -2240,19 +2882,55 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Science" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Engineering" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="6">
-    <chartFormat chart="0" format="2" series="1">
+  <chartFormats count="11">
+    <chartFormat chart="0" format="9" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="1" selected="0">
+          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2264,31 +2942,19 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="5" series="1">
+    <chartFormat chart="0" format="15" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
-            <x v="1"/>
+            <x v="4"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7" series="1">
+    <chartFormat chart="0" format="16" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2300,14 +2966,44 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
+    <chartFormat chart="0" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="19" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
-            <x v="4"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -2585,166 +3281,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G9"/>
+  <dimension ref="A4:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>1980</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="5">
         <v>5.2631578947368397E-2</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.215053763440859</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.20481927710844E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2.90102389078498E-2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>5.9629248197713702E-2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.36837302226487528</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="C6" s="5">
+        <v>5.3763440860214902E-2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2.4096385542168798E-3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8.5324232081911405E-3</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1.59629248197674E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.13330000638975872</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>1990</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.22267871815940801</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.10913500404203701</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3.2454245765601797E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4.2292162749767E-2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>7.1468297581152695E-2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.47802842829796649</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="B7" s="5">
+        <v>4.1906327033689302E-2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>5.86095392077607E-2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4.8880300102307501E-3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>9.2142043689822893E-3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1.5999741847800501E-2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.13061784246846356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>2000</v>
       </c>
-      <c r="B7" s="1">
-        <v>0.22991689750692501</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.25889594152721601</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2.5519152072795599E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4.8128342245989199E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <v>8.5853952535626402E-2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.64831428588855222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="B8" s="5">
+        <v>5.8171745152354501E-2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>6.4243123677630201E-2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2.5671656965660901E-3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5.4140233168366103E-3</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1.51227615776199E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.14551881942100731</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>2010</v>
       </c>
-      <c r="B8" s="1">
-        <v>0.256354916067146</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.25489675516224197</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2.2189234324657199E-2</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4.9482872314580102E-2</v>
-      </c>
-      <c r="F8" s="1">
-        <v>8.13973065688815E-2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.66432108443750693</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.76158211068084747</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.83798146417235397</v>
-      </c>
-      <c r="D9" s="1">
-        <v>9.2210824934138985E-2</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.1689136162181861</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.29834880488337429</v>
-      </c>
-      <c r="G9" s="1">
-        <v>2.1590368208889008</v>
+      <c r="B9" s="5">
+        <v>2.90167865707434E-2</v>
+      </c>
+      <c r="C9" s="5">
+        <v>5.0412979351032401E-2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2.0512474485923E-3</v>
+      </c>
+      <c r="E9" s="5">
+        <v>7.4272029986464398E-3</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1.1792474943997201E-2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.10070069131301174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.18172643770415559</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.22702908309663822</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.191608170960602E-2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3.0587853892656478E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5.887790318918501E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.51013735959224138</v>
       </c>
     </row>
   </sheetData>
@@ -2755,15 +3457,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D21"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2776,285 +3481,903 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>0.74110405847278304</v>
-      </c>
-      <c r="D2">
-        <v>0.25889594152721601</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5.4140233168366103E-3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9.6655262895672008E-3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.12575148636529E-3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.2552894675656798E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6.8422625967382899E-3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.27398943767230099</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.67941010396253398</v>
+      </c>
+      <c r="J2" s="2">
+        <f>SUM(C2:I2)</f>
+        <v>0.99999999999999911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>0.91414604746440398</v>
-      </c>
-      <c r="D3">
-        <v>8.5853952535626402E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.5671656965660901E-3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.50761253590219E-3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9.4044683933609396E-4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.29629158935515E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.8213405180082798E-3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.556566606511958</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.42063391200467698</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J21" si="0">SUM(C3:I3)</f>
+        <v>0.99999999999999911</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>0.77008310249307399</v>
-      </c>
-      <c r="D4">
-        <v>0.22991689750692501</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.8171745152354501E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.5401662049861501E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3.7857802400738598E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7.8485687903970397E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.140350877192982</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.62973222530009199</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.999999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2000</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>0.95187165775401095</v>
-      </c>
-      <c r="D5">
-        <v>4.8128342245989199E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6.4243123677630201E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.94345066358914E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.5204847085977999E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.1159838430467299E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.5391421427197499E-2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.129832660126947</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.61473360261588705</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999845</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2000</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>0.97448084792720402</v>
-      </c>
-      <c r="D6">
-        <v>2.5519152072795599E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.51227615776199E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.69499283819281E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4.8864314745695799E-3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3.8641335548313699E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7.4269180960085598E-3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.25538947452743299</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.66158315039417903</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="0"/>
+        <v>1.000000000000052</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2010</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>0.743645083932853</v>
-      </c>
-      <c r="D7">
-        <v>0.256354916067146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.4272029986464398E-3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.41646131954326E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.2255579078887902E-3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.8611390691701601E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3.4576406483184598E-3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.24626904522264201</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.70784454933537</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2010</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>0.918602693431118</v>
-      </c>
-      <c r="D8">
-        <v>8.13973065688815E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.0512474485923E-3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.0802449351394201E-3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.1996929876351599E-3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.04350466422631E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2.7226261365361601E-3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.48588249186080001</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.49362864998903599</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2010</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>0.74510324483775703</v>
-      </c>
-      <c r="D9">
-        <v>0.25489675516224197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5.0412979351032401E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.68141592920354E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.2743362831858399E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7.2654867256637196E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3.88200589970501E-2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.102300884955752</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.64625368731563404</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999956</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2010</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>0.95051712768541996</v>
-      </c>
-      <c r="D10">
-        <v>4.9482872314580102E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.90167865707434E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7.9136690647481994E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.45083932853717E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8.7170263788968805E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4.0407673860911202E-2</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2.1942446043165399E-2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.72781774580335701</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2010</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>0.97781076567534297</v>
-      </c>
-      <c r="D11">
-        <v>2.2189234324657199E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.1792474943997201E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.8125931255745398E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4.04157349862718E-3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.7328093501643698E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>7.5637840118548197E-3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.23254090391173199</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.68860723887639297</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>1990</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9.2142043689822893E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.0541463919660401E-3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3.7270939020602502E-3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.6150740242261E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>6.9883010663629704E-3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.32767367222279697</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.63319184180556898</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999845</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1990</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4.8880300102307501E-3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.9324769807889E-3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>7.4457201318631197E-3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.4209389564624199E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5.1153802432647396E-4</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.52728202796407697</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.44373081732408698</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999734</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1990</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4.1906327033689302E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.04026294165981E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2.3829087921117501E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>9.2851273623664701E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3.3689400164338502E-2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>4.51930977814297E-2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.73212818405916102</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999889</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1990</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5.86095392077607E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.5869037995149499E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2.8294260307194798E-3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.4955537590945801E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>6.8714632174616003E-3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.22837510105092901</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.66248989490703303</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999911</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1990</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.5999741847800501E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8.5304116578497503E-3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3.84001397058968E-3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3.2124763439574801E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>6.0836602944834102E-3</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.27618678830190801</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.65723462048779602</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>1980</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>0.94736842105263097</v>
-      </c>
-      <c r="D12">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8.5324232081911405E-3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.7064846416382201E-3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.0238907849829299E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>6.8259385665529098E-3</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.42832764505119297</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.54436860068259096</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1980</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.4096385542168798E-3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>7.2289156626506503E-3</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.56144578313253102</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.42891566265060399</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000027</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1980</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5.3763440860214902E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2.1505376344085898E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5.3763440860214902E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4.3010752688171901E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2.1505376344085898E-2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.18279569892472999</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.62365591397849396</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999745</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1980</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1">
         <v>5.2631578947368397E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>1980</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>0.94037075180224305</v>
-      </c>
-      <c r="D13">
-        <v>5.9629248197713702E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.59629248197674E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4.3769309989685297E-3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3.2440782698237298E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2.6210092687940698E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>8.1359423274944397E-3</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.310092687950418</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.63197734294527796</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999969069</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>3002872.18</v>
+      </c>
+      <c r="C22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>3924070.82</v>
+      </c>
+      <c r="C23">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>108018.42</v>
+      </c>
+      <c r="C24">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>518548.26</v>
+      </c>
+      <c r="C25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>52294579.659997799</v>
+      </c>
+      <c r="C26">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>4603164.88</v>
+      </c>
+      <c r="C27">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>5919207.8499999801</v>
+      </c>
+      <c r="C28">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>676982.99999999895</v>
+      </c>
+      <c r="C29">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>166549.799999999</v>
+      </c>
+      <c r="C30">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <v>48986509.850000098</v>
+      </c>
+      <c r="C31">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>1941265.82</v>
+      </c>
+      <c r="C32">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>1768021.06</v>
+      </c>
+      <c r="C33">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>122296.33</v>
+      </c>
+      <c r="C34">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>248612.25999999899</v>
+      </c>
+      <c r="C35">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36">
+        <v>52940242.289999202</v>
+      </c>
+      <c r="C36">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>1174695.5999999901</v>
+      </c>
+      <c r="C37">
         <v>1980</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>0.78494623655913898</v>
-      </c>
-      <c r="D14">
-        <v>0.215053763440859</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>831908.99999999395</v>
+      </c>
+      <c r="C38">
         <v>1980</v>
       </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>0.97098976109214796</v>
-      </c>
-      <c r="D15">
-        <v>2.90102389078498E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>186427.8</v>
+      </c>
+      <c r="C39">
         <v>1980</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <v>0.98795180722891496</v>
-      </c>
-      <c r="D16">
-        <v>1.20481927710844E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1990</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>0.89086499595796298</v>
-      </c>
-      <c r="D17">
-        <v>0.10913500404203701</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1990</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18">
-        <v>0.92853170241884198</v>
-      </c>
-      <c r="D18">
-        <v>7.1468297581152695E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1990</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19">
-        <v>0.77732128184059102</v>
-      </c>
-      <c r="D19">
-        <v>0.22267871815940801</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1990</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>0.95770783725023201</v>
-      </c>
-      <c r="D20">
-        <v>4.2292162749767E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1990</v>
-      </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21">
-        <v>0.96754575423439804</v>
-      </c>
-      <c r="D21">
-        <v>3.2454245765601797E-2</v>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40">
+        <v>38087.3999999999</v>
+      </c>
+      <c r="C40">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>38929332.000014201</v>
+      </c>
+      <c r="C41">
+        <v>1980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>